<commit_message>
First implementation of db writer
</commit_message>
<xml_diff>
--- a/excel_to_database/test/assets/practice.xlsx
+++ b/excel_to_database/test/assets/practice.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">نام خانوادگی</t>
   </si>
   <si>
-    <t xml:space="preserve">کد ملی </t>
+    <t xml:space="preserve">کد ملی</t>
   </si>
   <si>
     <t xml:space="preserve">محمد</t>
@@ -156,13 +156,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -194,7 +191,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2373456567</v>
+        <v>3610096152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing excel reader validation
</commit_message>
<xml_diff>
--- a/excel_to_database/test/assets/practice.xlsx
+++ b/excel_to_database/test/assets/practice.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">نام</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">علی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نامعتبر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نامعتبریان</t>
   </si>
 </sst>
 </file>
@@ -153,13 +159,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -184,11 +193,22 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>3610096152</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>